<commit_message>
Bruh Darren is inconsistent
</commit_message>
<xml_diff>
--- a/record.xlsx
+++ b/record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sovie\Documents\GitHub\Sleep-Paralysis-Demon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A10F3EF-9FFB-40F5-8742-5451BBEA1626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C7721-F143-4183-9B83-2324C0D9C4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Point" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="289">
   <si>
     <t>date</t>
   </si>
@@ -841,9 +841,6 @@
   </si>
   <si>
     <t>01:01:00</t>
-  </si>
-  <si>
-    <t>------</t>
   </si>
   <si>
     <t>02:06:00</t>
@@ -939,12 +936,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
@@ -2565,7 +2561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -2696,7 +2692,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -2723,9 +2719,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,19 +2754,19 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G2" s="3"/>
@@ -2779,19 +2775,19 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G3" s="3"/>
@@ -2800,19 +2796,19 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G4" s="3"/>
@@ -2821,19 +2817,19 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="2" t="s">
         <v>94</v>
       </c>
       <c r="G5" s="3"/>
@@ -2842,19 +2838,19 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>98</v>
       </c>
       <c r="G6" s="3"/>
@@ -2863,19 +2859,19 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G7" s="3"/>
@@ -2884,19 +2880,19 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G8" s="3"/>
@@ -2905,19 +2901,19 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="3"/>
@@ -2926,19 +2922,19 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="2" t="s">
         <v>83</v>
       </c>
       <c r="G10" s="3"/>
@@ -2947,19 +2943,19 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>119</v>
       </c>
       <c r="G11" s="3"/>
@@ -2968,19 +2964,19 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>123</v>
       </c>
       <c r="G12" s="3"/>
@@ -2989,19 +2985,19 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G13" s="3"/>
@@ -3010,19 +3006,19 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="2" t="s">
         <v>129</v>
       </c>
       <c r="G14" s="3"/>
@@ -3031,19 +3027,19 @@
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="2" t="s">
         <v>134</v>
       </c>
       <c r="G15" s="3"/>
@@ -3052,19 +3048,19 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>137</v>
       </c>
       <c r="G16" s="3"/>
@@ -3073,19 +3069,19 @@
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>140</v>
       </c>
       <c r="G17" s="3"/>
@@ -3094,19 +3090,19 @@
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="2" t="s">
         <v>144</v>
       </c>
       <c r="G18" s="3"/>
@@ -3115,19 +3111,19 @@
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="2" t="s">
         <v>148</v>
       </c>
       <c r="G19" s="3"/>
@@ -3136,19 +3132,19 @@
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="2" t="s">
         <v>152</v>
       </c>
       <c r="G20" s="3"/>
@@ -3157,19 +3153,19 @@
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="2" t="s">
         <v>153</v>
       </c>
       <c r="G21" s="3"/>
@@ -3178,19 +3174,19 @@
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="2" t="s">
         <v>156</v>
       </c>
       <c r="G22" s="3"/>
@@ -3199,19 +3195,19 @@
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G23" s="3"/>
@@ -3220,19 +3216,19 @@
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>150</v>
       </c>
       <c r="G24" s="3"/>
@@ -3241,19 +3237,19 @@
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G25" s="3"/>
@@ -3262,19 +3258,19 @@
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="2" t="s">
         <v>167</v>
       </c>
       <c r="G26" s="3"/>
@@ -3283,19 +3279,19 @@
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G27" s="3"/>
@@ -3304,19 +3300,19 @@
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="2" t="s">
         <v>131</v>
       </c>
       <c r="G28" s="3"/>
@@ -3325,19 +3321,19 @@
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F29" s="2" t="s">
         <v>176</v>
       </c>
       <c r="G29" s="3"/>
@@ -3346,19 +3342,19 @@
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="2" t="s">
         <v>179</v>
       </c>
       <c r="G30" s="3"/>
@@ -3367,19 +3363,19 @@
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="2" t="s">
         <v>180</v>
       </c>
       <c r="G31" s="3"/>
@@ -3388,19 +3384,19 @@
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="2" t="s">
         <v>182</v>
       </c>
       <c r="G32" s="3"/>
@@ -3409,19 +3405,19 @@
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="2" t="s">
         <v>135</v>
       </c>
       <c r="G33" s="3"/>
@@ -3430,19 +3426,19 @@
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="2" t="s">
         <v>144</v>
       </c>
       <c r="G34" s="3"/>
@@ -3451,19 +3447,19 @@
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="2" t="s">
         <v>189</v>
       </c>
       <c r="G35" s="3"/>
@@ -3472,19 +3468,19 @@
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="2" t="s">
         <v>90</v>
       </c>
       <c r="G36" s="3"/>
@@ -3493,19 +3489,19 @@
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="2" t="s">
         <v>195</v>
       </c>
       <c r="G37" s="3"/>
@@ -3514,19 +3510,19 @@
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="F38" s="2" t="s">
         <v>103</v>
       </c>
       <c r="G38" s="3"/>
@@ -3535,19 +3531,19 @@
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="2" t="s">
         <v>201</v>
       </c>
       <c r="G39" s="3"/>
@@ -3556,19 +3552,19 @@
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="2" t="s">
         <v>204</v>
       </c>
       <c r="G40" s="3"/>
@@ -3577,19 +3573,19 @@
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="2" t="s">
         <v>207</v>
       </c>
       <c r="G41" s="3"/>
@@ -3598,19 +3594,19 @@
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="2" t="s">
         <v>210</v>
       </c>
       <c r="G42" s="3"/>
@@ -3619,19 +3615,19 @@
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="E43" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="2" t="s">
         <v>174</v>
       </c>
       <c r="G43" s="3"/>
@@ -3640,19 +3636,19 @@
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="F44" s="4" t="s">
+      <c r="F44" s="2" t="s">
         <v>101</v>
       </c>
       <c r="G44" s="3"/>
@@ -3661,19 +3657,19 @@
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="F45" s="2" t="s">
         <v>217</v>
       </c>
       <c r="G45" s="3"/>
@@ -3682,19 +3678,19 @@
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="2" t="s">
         <v>221</v>
       </c>
       <c r="G46" s="3"/>
@@ -3703,19 +3699,19 @@
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="E47" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="2" t="s">
         <v>163</v>
       </c>
       <c r="G47" s="3"/>
@@ -3724,19 +3720,19 @@
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="E48" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="F48" s="2" t="s">
         <v>150</v>
       </c>
       <c r="G48" s="3"/>
@@ -3745,19 +3741,19 @@
       <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="E49" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F49" s="4" t="s">
+      <c r="F49" s="2" t="s">
         <v>163</v>
       </c>
       <c r="G49" s="3"/>
@@ -3766,19 +3762,19 @@
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="E50" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="F50" s="2" t="s">
         <v>230</v>
       </c>
       <c r="G50" s="3"/>
@@ -3787,19 +3783,19 @@
       <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="E51" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="F51" s="4" t="s">
+      <c r="F51" s="2" t="s">
         <v>232</v>
       </c>
       <c r="G51" s="3"/>
@@ -3808,19 +3804,19 @@
       <c r="A52" s="2">
         <v>51</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E52" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G52" s="3"/>
@@ -3829,19 +3825,19 @@
       <c r="A53" s="2">
         <v>52</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="E53" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F53" s="2" t="s">
         <v>111</v>
       </c>
       <c r="G53" s="3"/>
@@ -3850,19 +3846,19 @@
       <c r="A54" s="2">
         <v>53</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="E54" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="2" t="s">
         <v>238</v>
       </c>
       <c r="G54" s="3"/>
@@ -3871,19 +3867,19 @@
       <c r="A55" s="2">
         <v>54</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E55" s="4" t="s">
+      <c r="E55" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F55" s="2" t="s">
         <v>172</v>
       </c>
       <c r="G55" s="3"/>
@@ -3892,19 +3888,19 @@
       <c r="A56" s="2">
         <v>55</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="2" t="s">
         <v>162</v>
       </c>
       <c r="G56" s="3"/>
@@ -3913,19 +3909,19 @@
       <c r="A57" s="2">
         <v>56</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="E57" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="2" t="s">
         <v>241</v>
       </c>
       <c r="G57" s="3"/>
@@ -3934,19 +3930,19 @@
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E58" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="F58" s="4" t="s">
+      <c r="F58" s="2" t="s">
         <v>244</v>
       </c>
       <c r="G58" s="3"/>
@@ -3955,19 +3951,19 @@
       <c r="A59" s="2">
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E59" s="4" t="s">
+      <c r="E59" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="F59" s="4" t="s">
+      <c r="F59" s="2" t="s">
         <v>132</v>
       </c>
       <c r="G59" s="3"/>
@@ -3976,19 +3972,19 @@
       <c r="A60" s="2">
         <v>59</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E60" s="4" t="s">
+      <c r="E60" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="F60" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G60" s="3"/>
@@ -3997,19 +3993,19 @@
       <c r="A61" s="2">
         <v>60</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="4" t="s">
+      <c r="E61" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F61" s="4" t="s">
+      <c r="F61" s="2" t="s">
         <v>251</v>
       </c>
       <c r="G61" s="3"/>
@@ -4018,19 +4014,19 @@
       <c r="A62" s="2">
         <v>61</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E62" s="4" t="s">
+      <c r="E62" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="F62" s="4" t="s">
+      <c r="F62" s="2" t="s">
         <v>145</v>
       </c>
       <c r="G62" s="3"/>
@@ -4039,19 +4035,19 @@
       <c r="A63" s="2">
         <v>62</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="E63" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="F63" s="2" t="s">
         <v>256</v>
       </c>
       <c r="G63" s="3"/>
@@ -4060,19 +4056,19 @@
       <c r="A64" s="2">
         <v>63</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E64" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F64" s="4" t="s">
+      <c r="F64" s="2" t="s">
         <v>258</v>
       </c>
       <c r="G64" s="3"/>
@@ -4081,19 +4077,19 @@
       <c r="A65" s="2">
         <v>64</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E65" s="4" t="s">
+      <c r="E65" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="F65" s="4" t="s">
+      <c r="F65" s="2" t="s">
         <v>162</v>
       </c>
       <c r="G65" s="3"/>
@@ -4102,19 +4098,19 @@
       <c r="A66" s="2">
         <v>65</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E66" s="4" t="s">
+      <c r="E66" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F66" s="4" t="s">
+      <c r="F66" s="2" t="s">
         <v>261</v>
       </c>
       <c r="G66" s="3"/>
@@ -4123,19 +4119,19 @@
       <c r="A67" s="2">
         <v>66</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="2" t="s">
         <v>264</v>
       </c>
       <c r="G67" s="3"/>
@@ -4144,382 +4140,382 @@
       <c r="A68" s="2">
         <v>67</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E68" s="4" t="s">
+      <c r="E68" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F68" s="2" t="s">
         <v>174</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="4">
+      <c r="A69" s="2">
         <v>68</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C69" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E69" s="4" t="s">
+      <c r="E69" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F69" s="4" t="s">
+      <c r="F69" s="2" t="s">
         <v>170</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="4">
+      <c r="A70" s="2">
         <v>69</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="E70" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="F70" s="2" t="s">
         <v>253</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="4">
+      <c r="A71" s="2">
         <v>70</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="C71" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="E71" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="F71" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="4">
+      <c r="A72" s="2">
         <v>71</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="E72" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="F72" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="4">
+      <c r="A73" s="2">
         <v>72</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="C73" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="F73" s="2" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="4">
+      <c r="A74" s="2">
         <v>73</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D74" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F74" s="4" t="s">
+      <c r="C76" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A75" s="4">
-        <v>74</v>
-      </c>
-      <c r="B75" s="4" t="s">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
         <v>84</v>
       </c>
-      <c r="C75" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A76" s="4">
-        <v>75</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A77" s="4">
-        <v>76</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A78" s="4">
-        <v>77</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A79" s="4">
-        <v>78</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A80" s="4">
-        <v>79</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4">
-        <v>80</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4">
-        <v>81</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4">
-        <v>82</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4">
-        <v>83</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="F84" s="4" t="s">
+      <c r="B85" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="4">
-        <v>84</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="E85" s="4" t="s">
+      <c r="E85" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="F85" s="2" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="4">
+      <c r="A86" s="2">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4">
+      <c r="A87" s="2">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4">
+      <c r="A88" s="2">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="4">
+      <c r="A89" s="2">
         <v>88</v>
       </c>
     </row>

</xml_diff>